<commit_message>
padding to description text
</commit_message>
<xml_diff>
--- a/Parker and Benton List.xlsx
+++ b/Parker and Benton List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\VIP LIST FOR CR DE MILL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0451A9-32EA-412E-AF6D-3CEEB4454A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9835178B-32C8-474D-9A8E-8119C43EAEDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0F680B8A-8E70-49F5-8032-52E949A86C0A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="119">
   <si>
     <t>Buyer</t>
   </si>
@@ -125,9 +125,6 @@
     <t>phillip.gonzales2002@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Nick Proen </t>
-  </si>
-  <si>
     <t xml:space="preserve">Benton </t>
   </si>
   <si>
@@ -321,6 +318,78 @@
   </si>
   <si>
     <t>(408)569-2911</t>
+  </si>
+  <si>
+    <t>Maila Baker</t>
+  </si>
+  <si>
+    <t>rene_martin@hotmail.com</t>
+  </si>
+  <si>
+    <t>510-754-6886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryan and Adele Fields </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adelefields12@gmail.com </t>
+  </si>
+  <si>
+    <t>Ryanfields12@gmail.com</t>
+  </si>
+  <si>
+    <t>443-509-2084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead sent from Kevin estates </t>
+  </si>
+  <si>
+    <t>tienken@me.com</t>
+  </si>
+  <si>
+    <t>559-790-1632</t>
+  </si>
+  <si>
+    <t>Eric and Jane Tienken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colby and Nicole Linder </t>
+  </si>
+  <si>
+    <t>Parker lot 27</t>
+  </si>
+  <si>
+    <t>linder.family@yahoo.com</t>
+  </si>
+  <si>
+    <t>Dominic Dinnocenti</t>
+  </si>
+  <si>
+    <t>dominicdi@comcast.net</t>
+  </si>
+  <si>
+    <t>Golf course Parker</t>
+  </si>
+  <si>
+    <t>Brian and Kristine Goerlich</t>
+  </si>
+  <si>
+    <t>Beonton Lot 48</t>
+  </si>
+  <si>
+    <t>stirbee@comcast.net</t>
+  </si>
+  <si>
+    <t>Robert and Dolores Davis</t>
+  </si>
+  <si>
+    <t>rdaviscpa@hotmail.com</t>
+  </si>
+  <si>
+    <t>ddlove5@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nick and Courtney Proen </t>
   </si>
 </sst>
 </file>
@@ -756,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420005EE-D5B2-4098-BD44-06AA8EF6AEF0}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,6 +839,7 @@
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -927,27 +997,27 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -957,17 +1027,17 @@
         <v>19</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -977,19 +1047,19 @@
         <v>19</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -998,20 +1068,20 @@
       <c r="F11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>42</v>
+      <c r="G11" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1021,95 +1091,95 @@
         <v>19</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="4">
         <v>5596799500</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="4">
         <v>5597909791</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="9">
@@ -1119,167 +1189,167 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="4"/>
@@ -1287,7 +1357,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1297,27 +1367,116 @@
         <v>11</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+      <c r="F26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="I26" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1332,7 +1491,7 @@
     <hyperlink ref="I9" r:id="rId9" display="tel:559-297-1950" xr:uid="{4216ED26-2A3E-4BD6-BB3D-E6F0667A8188}"/>
     <hyperlink ref="G10" r:id="rId10" display="mailto:ginabadams@comcast.net" xr:uid="{FD944A6E-B50B-4A48-AAF4-A439FEDD2D57}"/>
     <hyperlink ref="I10" r:id="rId11" display="tel:559-930-5272" xr:uid="{3FB8F821-3BF4-4303-8776-38E51709532F}"/>
-    <hyperlink ref="G11" r:id="rId12" display="mailto:ahensleit@yahoo.com" xr:uid="{7045AF32-33F5-4688-A9B4-BF739BA89961}"/>
+    <hyperlink ref="G11" r:id="rId12" xr:uid="{7045AF32-33F5-4688-A9B4-BF739BA89961}"/>
     <hyperlink ref="G12" r:id="rId13" display="mailto:imdanjang@yahoo.com" xr:uid="{94390787-78D3-45B8-B285-335440B7C7D6}"/>
     <hyperlink ref="G13" r:id="rId14" display="mailto:kmbeshore@gmail.com" xr:uid="{94CE5A72-0F76-455B-BFB6-B12DF0B5B36E}"/>
     <hyperlink ref="G14" r:id="rId15" xr:uid="{3AFD0F83-1DD2-4CB8-892D-F1D509B93D83}"/>
@@ -1351,8 +1510,17 @@
     <hyperlink ref="G8" r:id="rId28" xr:uid="{C9E5B0C8-AA31-4812-BCF9-7282B91353EA}"/>
     <hyperlink ref="G23" r:id="rId29" xr:uid="{59B703CB-78B4-4B21-90F7-B8FD2FBDBB73}"/>
     <hyperlink ref="G20" r:id="rId30" xr:uid="{EE17C20D-4FEB-4908-A133-1722B528A8EA}"/>
+    <hyperlink ref="G26" r:id="rId31" display="mailto:rene_martin@hotmail.com" xr:uid="{0A39A7CB-6898-4FE8-8B3A-8ABFA52F2C17}"/>
+    <hyperlink ref="G27" r:id="rId32" display="mailto:adelefields12@gmail.com" xr:uid="{EFF6F00F-D281-4EE9-B683-494B223FD602}"/>
+    <hyperlink ref="H27" r:id="rId33" xr:uid="{376A9E40-3214-4C91-A4D2-20415DD27986}"/>
+    <hyperlink ref="G28" r:id="rId34" display="mailto:tienken@me.com" xr:uid="{F4F71E11-0144-4CC8-BF05-232BD508B24D}"/>
+    <hyperlink ref="G29" r:id="rId35" xr:uid="{835A00E3-F6F1-4E5F-BD82-936CE856E49A}"/>
+    <hyperlink ref="G30" r:id="rId36" xr:uid="{00C08A21-39EF-45A1-B6BC-DE4F09D21327}"/>
+    <hyperlink ref="G31" r:id="rId37" xr:uid="{8C96BA66-9C84-41E0-A0B9-7DF4D6BCFD9F}"/>
+    <hyperlink ref="G32" r:id="rId38" xr:uid="{97DC6602-0E97-454E-A0B2-02B591953D7F}"/>
+    <hyperlink ref="H32" r:id="rId39" xr:uid="{B5F76AB2-DD50-4698-A890-EC4D7FCC3DB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>